<commit_message>
this is my second commit
</commit_message>
<xml_diff>
--- a/Testdata/DocData.xlsx
+++ b/Testdata/DocData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="40">
   <si>
     <t>Dr. Sivakumar Mahalingam</t>
   </si>
@@ -504,7 +504,7 @@
         <v>26</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
@@ -520,7 +520,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>